<commit_message>
added labels for effort
</commit_message>
<xml_diff>
--- a/MasterCountSheet.xlsx
+++ b/MasterCountSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejnic\Documents\BONWRAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E39D6E7-B6AE-4B7B-853C-87E9981FC19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C628B19-2854-474E-B3B3-21CB5414FE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{2C8658AB-1D65-4586-B8E3-CBCB320D0820}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="229">
   <si>
     <t>Pipevine Swallowtail</t>
   </si>
@@ -705,6 +705,24 @@
   </si>
   <si>
     <t>Common Name</t>
+  </si>
+  <si>
+    <t>Total Species *</t>
+  </si>
+  <si>
+    <t>Total Individuals</t>
+  </si>
+  <si>
+    <t>Observers</t>
+  </si>
+  <si>
+    <t>Party Hours</t>
+  </si>
+  <si>
+    <t>Number of Parties</t>
+  </si>
+  <si>
+    <t>Count Date</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1120,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A49DBB-E3C7-4F3C-B8AD-9EA7CC829232}">
   <dimension ref="A1:Y86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5446,6 +5466,9 @@
       </c>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>223</v>
+      </c>
       <c r="F80">
         <v>41</v>
       </c>
@@ -5504,7 +5527,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="81" spans="6:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>224</v>
+      </c>
       <c r="F81">
         <v>947</v>
       </c>
@@ -5563,7 +5589,10 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="83" spans="6:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>225</v>
+      </c>
       <c r="F83">
         <v>7</v>
       </c>
@@ -5619,7 +5648,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="6:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>226</v>
+      </c>
       <c r="F84">
         <v>8</v>
       </c>
@@ -5675,7 +5707,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E85" t="s">
+        <v>227</v>
+      </c>
       <c r="F85">
         <v>1</v>
       </c>
@@ -5731,7 +5766,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E86" t="s">
+        <v>228</v>
+      </c>
       <c r="F86" s="1">
         <v>45890</v>
       </c>

</xml_diff>